<commit_message>
Creature Inheritance tree diagram Image
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7E25F1-D80E-4ABC-B7C7-0D72DDE646DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD8864C-B112-458B-B226-055CD75301D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Inheritance tree diagram</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Status</t>
   </si>
@@ -106,6 +103,12 @@
   </si>
   <si>
     <t>show handling of user input</t>
+  </si>
+  <si>
+    <t>Creature Inheritance tree diagram</t>
+  </si>
+  <si>
+    <t>Creature Inheritance Drawing.png</t>
   </si>
 </sst>
 </file>
@@ -121,12 +124,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -174,11 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +472,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,133 +482,137 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DisplayEnumerable, ShowTurnDecisions, GetWeapons, GetSpells
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD8864C-B112-458B-B226-055CD75301D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5440F7B-BE3F-4694-A07B-85CF7BBF74A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Status</t>
   </si>
@@ -109,6 +109,33 @@
   </si>
   <si>
     <t>Creature Inheritance Drawing.png</t>
+  </si>
+  <si>
+    <t>virtual Monster.GetAttackMessage.png</t>
+  </si>
+  <si>
+    <t>override Shulker.GetAttackMessage.png</t>
+  </si>
+  <si>
+    <t>override Dragon.GetAttackMessage.png</t>
+  </si>
+  <si>
+    <t>override Skeleton.GetAttackMessage.png</t>
+  </si>
+  <si>
+    <t>override Warden.GetAttackMessage.png</t>
+  </si>
+  <si>
+    <t>override Witch.GetAttackMessage.png</t>
+  </si>
+  <si>
+    <t>UserInterface.ShowTurnDecisions.png</t>
+  </si>
+  <si>
+    <t>UserInterface.DisplayEnumerable Weapons.png</t>
+  </si>
+  <si>
+    <t>UserInterface.DisplayEnumerable.png</t>
   </si>
 </sst>
 </file>
@@ -469,18 +496,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>26</v>
@@ -500,72 +532,102 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Inventory list of type item
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA1D34-678D-4104-ACBA-C254FD776DD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAAFDB5-B05C-4F0C-90A9-8457E8E9CC1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +611,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
User displaying the players inventory.png
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAAFDB5-B05C-4F0C-90A9-8457E8E9CC1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6DF49-5220-4D3D-A980-D2EF3D3BD503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Item Inheritance Drawing.png</t>
+  </si>
+  <si>
+    <t>User displaying the players inventory.png</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,8 +629,12 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Weapons In Inventory, Sort Weapons Screenshots
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6DF49-5220-4D3D-A980-D2EF3D3BD503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9855960-C310-43BD-91A3-77213011BCB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Status</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>User displaying the players inventory.png</t>
+  </si>
+  <si>
+    <t>User having the functionality to sort the damage of the weapons</t>
+  </si>
+  <si>
+    <t>User Sorted the weapons by descending damage</t>
+  </si>
+  <si>
+    <t>weapons in inventory.png</t>
+  </si>
+  <si>
+    <t>weapons sort by descending damage.png</t>
   </si>
 </sst>
 </file>
@@ -508,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,72 +650,90 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test for Positive Integer Screenshots
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E84DC6-681B-40D0-BC06-9E416ADBEFC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A87B45-067C-44EA-AD6A-3D90D8625592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Status</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>other tests class.png</t>
+  </si>
+  <si>
+    <t>Tests.TestForPositiveInteger.png</t>
+  </si>
+  <si>
+    <t>Tests that the mean is positive and std dev is above zero.png</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,8 +837,15 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="B27" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
User Input Error Handling
</commit_message>
<xml_diff>
--- a/Assessment Brief/Screenshots Required To Do List.xlsx
+++ b/Assessment Brief/Screenshots Required To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Module Dev Containers\CMP1903-Object-Oriented-Programming-A02\Assessment Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A87B45-067C-44EA-AD6A-3D90D8625592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD98FF28-01B0-4869-8B63-07D2179E9231}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,6 +849,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
       <c r="B28" s="3" t="s">
         <v>24</v>
       </c>

</xml_diff>